<commit_message>
Add new Dictionary endpoint for data-entry{CRUD}, admin-review, add tracking for each word: who's create when's create who's review and when's review.
</commit_message>
<xml_diff>
--- a/Notebook.xlsx
+++ b/Notebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phara\OneDrive\Desktop\Django_project\dictionary_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132ABAC3-A54E-4B8C-AA37-01137AF48223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2063B5B7-E0C4-4B77-ACFF-17A8C1079335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{486725EA-1341-4414-9EC0-725F2D77815B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>No</t>
   </si>
@@ -121,12 +121,22 @@
   </si>
   <si>
     <t>/users/detail/?{id/username/email}=</t>
+  </si>
+  <si>
+    <t>- User Suspend</t>
+  </si>
+  <si>
+    <t>not yet start</t>
   </si>
   <si>
     <t>- required FMIS mail
 - required role selection
 - required password to be 8 length, 1 uppercase, 1 lower case, 1 special character, 1 number
-- USER cannot perform this endpoint</t>
+- USER cannot perform this endpoint
+- Need to add who's register &amp; when's register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -249,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -268,9 +278,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -306,6 +313,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -648,16 +661,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{672CA8AB-C23A-439B-9906-9ACD271823D5}">
-  <dimension ref="J4:N30"/>
+  <dimension ref="J4:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31:M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="10" max="10" width="6.6640625" customWidth="1"/>
-    <col min="11" max="11" width="24.33203125" customWidth="1"/>
+    <col min="11" max="11" width="43.21875" customWidth="1"/>
     <col min="12" max="12" width="39.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.44140625" style="3" customWidth="1"/>
     <col min="14" max="14" width="8.88671875" style="6"/>
@@ -678,18 +691,18 @@
       </c>
     </row>
     <row r="5" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="11"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="10"/>
     </row>
     <row r="6" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J6" s="1">
         <v>1</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="20" t="s">
         <v>28</v>
       </c>
       <c r="L6" s="7" t="s">
@@ -697,13 +710,16 @@
       </c>
       <c r="M6" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J7" s="1">
         <v>2</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="20" t="s">
         <v>26</v>
       </c>
       <c r="L7" s="7" t="s">
@@ -717,7 +733,7 @@
       <c r="J8" s="1">
         <v>3</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="20" t="s">
         <v>5</v>
       </c>
       <c r="L8" s="5" t="s">
@@ -731,7 +747,7 @@
       <c r="J9" s="1">
         <v>4</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="20" t="s">
         <v>7</v>
       </c>
       <c r="L9" s="5" t="s">
@@ -741,227 +757,256 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="10:14" ht="147.6" x14ac:dyDescent="0.85">
+    <row r="10" spans="10:14" ht="196.8" x14ac:dyDescent="0.85">
       <c r="J10" s="1">
         <v>5</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="20" t="s">
         <v>6</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J11" s="1">
         <v>6</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="L11" s="7"/>
+      <c r="L11" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="M11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
-      <c r="J12" s="12" t="s">
+      <c r="J12" s="1">
+        <v>7</v>
+      </c>
+      <c r="K12" s="20"/>
+      <c r="L12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
+      <c r="J13" s="1"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
+      <c r="J14" s="1"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
+      <c r="J15" s="1"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
+      <c r="J16" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="14"/>
-    </row>
-    <row r="13" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
-      <c r="J13" s="1">
-        <v>1</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
-      <c r="J14" s="1">
-        <v>2</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
-      <c r="J15" s="1">
-        <v>3</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
-      <c r="J16" s="1">
-        <v>4</v>
-      </c>
-      <c r="K16" s="8"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="1"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="13"/>
     </row>
     <row r="17" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J17" s="1">
-        <v>5</v>
-      </c>
-      <c r="K17" s="8"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="K17" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="18" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J18" s="1">
-        <v>6</v>
-      </c>
-      <c r="K18" s="8"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="K18" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="19" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J19" s="1">
-        <v>7</v>
-      </c>
-      <c r="K19" s="8"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="K19" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="20" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
-      <c r="J20" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="17"/>
+      <c r="J20" s="1">
+        <v>4</v>
+      </c>
+      <c r="K20" s="20"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="1"/>
     </row>
     <row r="21" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J21" s="1">
-        <v>1</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="K21" s="20"/>
       <c r="L21" s="5"/>
-      <c r="M21" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="M21" s="1"/>
     </row>
     <row r="22" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J22" s="1">
-        <v>2</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="K22" s="20"/>
       <c r="L22" s="5"/>
-      <c r="M22" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="M22" s="1"/>
     </row>
     <row r="23" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J23" s="1">
-        <v>3</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="K23" s="20"/>
       <c r="L23" s="5"/>
-      <c r="M23" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="M23" s="1"/>
     </row>
     <row r="24" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
-      <c r="J24" s="1">
-        <v>4</v>
-      </c>
-      <c r="K24" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="L24" s="5"/>
-      <c r="M24" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="J24" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="16"/>
     </row>
     <row r="25" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J25" s="1">
-        <v>5</v>
-      </c>
-      <c r="K25" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="K25" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="L25" s="5"/>
-      <c r="M25" s="1"/>
+      <c r="M25" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="26" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J26" s="1">
-        <v>6</v>
-      </c>
-      <c r="K26" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="K26" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="L26" s="5"/>
-      <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="10:13" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="J27" s="18"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="20"/>
+      <c r="M26" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
+      <c r="J27" s="1">
+        <v>3</v>
+      </c>
+      <c r="K27" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="L27" s="5"/>
+      <c r="M27" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="28" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J28" s="1">
-        <v>1</v>
-      </c>
-      <c r="K28" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="K28" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="L28" s="5"/>
-      <c r="M28" s="1"/>
+      <c r="M28" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="29" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J29" s="1">
-        <v>2</v>
-      </c>
-      <c r="K29" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="K29" s="21"/>
       <c r="L29" s="5"/>
       <c r="M29" s="1"/>
     </row>
     <row r="30" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J30" s="1">
-        <v>3</v>
-      </c>
-      <c r="K30" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="K30" s="21"/>
       <c r="L30" s="5"/>
       <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="10:13" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="J31" s="17"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="19"/>
+    </row>
+    <row r="32" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
+      <c r="J32" s="1">
+        <v>1</v>
+      </c>
+      <c r="K32" s="21"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="1"/>
+    </row>
+    <row r="33" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
+      <c r="J33" s="1">
+        <v>2</v>
+      </c>
+      <c r="K33" s="21"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
+      <c r="J34" s="1">
+        <v>3</v>
+      </c>
+      <c r="K34" s="21"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="J5:M5"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J31:M31"/>
   </mergeCells>
-  <conditionalFormatting sqref="M1:M11 M13:M19 M21:M26 M28:M1048576">
+  <conditionalFormatting sqref="M17:M23 M25:M30 M32:M1048576 M1:M15">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="not yet start">
       <formula>NOT(ISERROR(SEARCH("not yet start",M1)))</formula>
     </cfRule>
@@ -973,7 +1018,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M13:M19 M6:M11 M21:M26 M28:M30" xr:uid="{0829E016-6B2C-4D31-BD7B-9AAAD991C688}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M17:M23 M25:M30 M32:M34 M6:M15" xr:uid="{0829E016-6B2C-4D31-BD7B-9AAAD991C688}">
       <formula1>"done, pending, not yet start"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Cleanup on Staging endpoints, also verify most of the endpoints except /sync & /sync_all. Other works fine. Also not yet optimize on indexing and reorganize on delete/reject data structure.
</commit_message>
<xml_diff>
--- a/Notebook.xlsx
+++ b/Notebook.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phara\OneDrive\Desktop\Django_project\dictionary_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phara\OneDrive\Desktop\FMIS\python\dictionary_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2063B5B7-E0C4-4B77-ACFF-17A8C1079335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A44082-A36D-4101-B157-37CD8CE8921D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{486725EA-1341-4414-9EC0-725F2D77815B}"/>
+    <workbookView xWindow="3984" yWindow="588" windowWidth="10980" windowHeight="11652" activeTab="1" xr2:uid="{486725EA-1341-4414-9EC0-725F2D77815B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="68">
   <si>
     <t>No</t>
   </si>
@@ -138,12 +139,117 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>GET /dictionary/bookmarks/</t>
+  </si>
+  <si>
+    <t>POST /dictionary/bookmarks/</t>
+  </si>
+  <si>
+    <t>DELETE /dictionary/bookmarks/</t>
+  </si>
+  <si>
+    <t>GET /dictionary/sync/</t>
+  </si>
+  <si>
+    <t>GET /dictionary/sync_all/</t>
+  </si>
+  <si>
+    <t>POST /users/mobile/login/</t>
+  </si>
+  <si>
+    <t>POST /users/mobile/refresh/</t>
+  </si>
+  <si>
+    <t>dictionary</t>
+  </si>
+  <si>
+    <t>GET /dictionary/list/</t>
+  </si>
+  <si>
+    <t>GET /dictionary/search/</t>
+  </si>
+  <si>
+    <t>POST /dictionary/staging/create/</t>
+  </si>
+  <si>
+    <t>GET /dictionary/staging/list/</t>
+  </si>
+  <si>
+    <t>GET /dictionary/staging/{id}/</t>
+  </si>
+  <si>
+    <t>POST /dictionary/staging/{id}/approve/</t>
+  </si>
+  <si>
+    <t>DELETE /dictionary/staging/{id}/delete/</t>
+  </si>
+  <si>
+    <t>POST /dictionary/staging/{id}/reject/</t>
+  </si>
+  <si>
+    <t>PUT /dictionary/staging/{id}/update/</t>
+  </si>
+  <si>
+    <t>GET /dictionary/{id}/</t>
+  </si>
+  <si>
+    <t>token</t>
+  </si>
+  <si>
+    <t>POST /token/</t>
+  </si>
+  <si>
+    <t>POST /token/blacklist/</t>
+  </si>
+  <si>
+    <t>POST /token/refresh/</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>GET /users/detail/</t>
+  </si>
+  <si>
+    <t>DELETE /users/drop/</t>
+  </si>
+  <si>
+    <t>GET /users/list/</t>
+  </si>
+  <si>
+    <t>POST /users/login/</t>
+  </si>
+  <si>
+    <t>POST /users/register/</t>
+  </si>
+  <si>
+    <t>PUT /users/update/</t>
+  </si>
+  <si>
+    <t>PATCH /users/update/</t>
+  </si>
+  <si>
+    <t>- now when perform reject, word delete from db but I want to keep all that word when user entry wheather user delete or admin reject. The point is I want to record all when user input The data</t>
+  </si>
+  <si>
+    <t>- need to update on indexing.</t>
+  </si>
+  <si>
+    <t>- need to record all data that have been delete or reject from admin.</t>
+  </si>
+  <si>
+    <t>- they want to keep deviceID so might save them all</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +267,23 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Khmer OS Siemreap"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Khmer OS Siemreap"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -195,7 +318,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -255,11 +378,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -278,6 +463,16 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -314,17 +509,159 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -663,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{672CA8AB-C23A-439B-9906-9ACD271823D5}">
   <dimension ref="J4:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31:M31"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,18 +1028,18 @@
       </c>
     </row>
     <row r="5" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="10"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="14"/>
     </row>
     <row r="6" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J6" s="1">
         <v>1</v>
       </c>
-      <c r="K6" s="20" t="s">
+      <c r="K6" s="8" t="s">
         <v>28</v>
       </c>
       <c r="L6" s="7" t="s">
@@ -719,7 +1056,7 @@
       <c r="J7" s="1">
         <v>2</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="K7" s="8" t="s">
         <v>26</v>
       </c>
       <c r="L7" s="7" t="s">
@@ -733,7 +1070,7 @@
       <c r="J8" s="1">
         <v>3</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="K8" s="8" t="s">
         <v>5</v>
       </c>
       <c r="L8" s="5" t="s">
@@ -747,7 +1084,7 @@
       <c r="J9" s="1">
         <v>4</v>
       </c>
-      <c r="K9" s="20" t="s">
+      <c r="K9" s="8" t="s">
         <v>7</v>
       </c>
       <c r="L9" s="5" t="s">
@@ -761,7 +1098,7 @@
       <c r="J10" s="1">
         <v>5</v>
       </c>
-      <c r="K10" s="20" t="s">
+      <c r="K10" s="8" t="s">
         <v>6</v>
       </c>
       <c r="L10" s="7" t="s">
@@ -775,7 +1112,7 @@
       <c r="J11" s="1">
         <v>6</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="K11" s="8" t="s">
         <v>27</v>
       </c>
       <c r="L11" s="7" t="s">
@@ -789,7 +1126,7 @@
       <c r="J12" s="1">
         <v>7</v>
       </c>
-      <c r="K12" s="20"/>
+      <c r="K12" s="8"/>
       <c r="L12" s="7" t="s">
         <v>29</v>
       </c>
@@ -799,35 +1136,35 @@
     </row>
     <row r="13" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J13" s="1"/>
-      <c r="K13" s="20"/>
+      <c r="K13" s="8"/>
       <c r="L13" s="7"/>
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J14" s="1"/>
-      <c r="K14" s="20"/>
+      <c r="K14" s="8"/>
       <c r="L14" s="7"/>
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J15" s="1"/>
-      <c r="K15" s="20"/>
+      <c r="K15" s="8"/>
       <c r="L15" s="7"/>
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="13"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="17"/>
     </row>
     <row r="17" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J17" s="1">
         <v>1</v>
       </c>
-      <c r="K17" s="20" t="s">
+      <c r="K17" s="8" t="s">
         <v>11</v>
       </c>
       <c r="L17" s="5" t="s">
@@ -841,7 +1178,7 @@
       <c r="J18" s="1">
         <v>2</v>
       </c>
-      <c r="K18" s="20" t="s">
+      <c r="K18" s="8" t="s">
         <v>12</v>
       </c>
       <c r="L18" s="5" t="s">
@@ -855,7 +1192,7 @@
       <c r="J19" s="1">
         <v>3</v>
       </c>
-      <c r="K19" s="20" t="s">
+      <c r="K19" s="8" t="s">
         <v>13</v>
       </c>
       <c r="L19" s="5" t="s">
@@ -869,7 +1206,7 @@
       <c r="J20" s="1">
         <v>4</v>
       </c>
-      <c r="K20" s="20"/>
+      <c r="K20" s="8"/>
       <c r="L20" s="5"/>
       <c r="M20" s="1"/>
     </row>
@@ -877,7 +1214,7 @@
       <c r="J21" s="1">
         <v>5</v>
       </c>
-      <c r="K21" s="20"/>
+      <c r="K21" s="8"/>
       <c r="L21" s="5"/>
       <c r="M21" s="1"/>
     </row>
@@ -885,7 +1222,7 @@
       <c r="J22" s="1">
         <v>6</v>
       </c>
-      <c r="K22" s="20"/>
+      <c r="K22" s="8"/>
       <c r="L22" s="5"/>
       <c r="M22" s="1"/>
     </row>
@@ -893,23 +1230,23 @@
       <c r="J23" s="1">
         <v>7</v>
       </c>
-      <c r="K23" s="20"/>
+      <c r="K23" s="8"/>
       <c r="L23" s="5"/>
       <c r="M23" s="1"/>
     </row>
     <row r="24" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
-      <c r="J24" s="14" t="s">
+      <c r="J24" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="16"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="20"/>
     </row>
     <row r="25" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J25" s="1">
         <v>1</v>
       </c>
-      <c r="K25" s="20" t="s">
+      <c r="K25" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L25" s="5"/>
@@ -921,7 +1258,7 @@
       <c r="J26" s="1">
         <v>2</v>
       </c>
-      <c r="K26" s="20" t="s">
+      <c r="K26" s="8" t="s">
         <v>16</v>
       </c>
       <c r="L26" s="5"/>
@@ -933,7 +1270,7 @@
       <c r="J27" s="1">
         <v>3</v>
       </c>
-      <c r="K27" s="20" t="s">
+      <c r="K27" s="8" t="s">
         <v>17</v>
       </c>
       <c r="L27" s="5"/>
@@ -945,7 +1282,7 @@
       <c r="J28" s="1">
         <v>4</v>
       </c>
-      <c r="K28" s="20" t="s">
+      <c r="K28" s="8" t="s">
         <v>18</v>
       </c>
       <c r="L28" s="5"/>
@@ -957,7 +1294,7 @@
       <c r="J29" s="1">
         <v>5</v>
       </c>
-      <c r="K29" s="21"/>
+      <c r="K29" s="9"/>
       <c r="L29" s="5"/>
       <c r="M29" s="1"/>
     </row>
@@ -965,21 +1302,21 @@
       <c r="J30" s="1">
         <v>6</v>
       </c>
-      <c r="K30" s="21"/>
+      <c r="K30" s="9"/>
       <c r="L30" s="5"/>
       <c r="M30" s="1"/>
     </row>
     <row r="31" spans="10:13" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="J31" s="17"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="19"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="23"/>
     </row>
     <row r="32" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J32" s="1">
         <v>1</v>
       </c>
-      <c r="K32" s="21"/>
+      <c r="K32" s="9"/>
       <c r="L32" s="5"/>
       <c r="M32" s="1"/>
     </row>
@@ -987,7 +1324,7 @@
       <c r="J33" s="1">
         <v>2</v>
       </c>
-      <c r="K33" s="21"/>
+      <c r="K33" s="9"/>
       <c r="L33" s="5"/>
       <c r="M33" s="1"/>
     </row>
@@ -995,7 +1332,7 @@
       <c r="J34" s="1">
         <v>3</v>
       </c>
-      <c r="K34" s="21"/>
+      <c r="K34" s="9"/>
       <c r="L34" s="5"/>
       <c r="M34" s="1"/>
     </row>
@@ -1006,14 +1343,14 @@
     <mergeCell ref="J24:M24"/>
     <mergeCell ref="J31:M31"/>
   </mergeCells>
-  <conditionalFormatting sqref="M17:M23 M25:M30 M32:M1048576 M1:M15">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="not yet start">
+  <conditionalFormatting sqref="M1:M15 M17:M23 M25:M30 M32:M1048576">
+    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="not yet start">
       <formula>NOT(ISERROR(SEARCH("not yet start",M1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pending">
+    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="pending">
       <formula>NOT(ISERROR(SEARCH("pending",M1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="done">
+    <cfRule type="containsText" dxfId="16" priority="3" operator="containsText" text="done">
       <formula>NOT(ISERROR(SEARCH("done",M1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1025,4 +1362,519 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F6179A3-1381-4E12-8A42-D0F2DF9F79BC}">
+  <dimension ref="B2:G39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="14.33203125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B2" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B4" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B5" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B6" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B7" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B8" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B9" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B10" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B11" s="24"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26"/>
+    </row>
+    <row r="12" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B12" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="26"/>
+    </row>
+    <row r="13" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B13" s="24"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="26"/>
+    </row>
+    <row r="14" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B14" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B15" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B16" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B17" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B18" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B19" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B20" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B21" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B22" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B23" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B24" s="24"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="26"/>
+    </row>
+    <row r="25" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B25" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="26"/>
+    </row>
+    <row r="26" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B26" s="24"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="26"/>
+    </row>
+    <row r="27" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B27" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B28" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B29" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B30" s="24"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="26"/>
+    </row>
+    <row r="31" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B31" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="26"/>
+    </row>
+    <row r="32" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B32" s="24"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="26"/>
+    </row>
+    <row r="33" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B33" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B34" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B35" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B36" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B37" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B38" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B39" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="38">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F4:F10">
+    <cfRule type="containsText" dxfId="15" priority="25" operator="containsText" text="error">
+      <formula>NOT(ISERROR(SEARCH("error",F4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="35" operator="containsText" text="not yet start">
+      <formula>NOT(ISERROR(SEARCH("not yet start",F4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="36" operator="containsText" text="pending">
+      <formula>NOT(ISERROR(SEARCH("pending",F4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="37" operator="containsText" text="done">
+      <formula>NOT(ISERROR(SEARCH("done",F4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14:F23">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="error">
+      <formula>NOT(ISERROR(SEARCH("error",F14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="not yet start">
+      <formula>NOT(ISERROR(SEARCH("not yet start",F14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="pending">
+      <formula>NOT(ISERROR(SEARCH("pending",F14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="done">
+      <formula>NOT(ISERROR(SEARCH("done",F14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27:F29">
+    <cfRule type="containsText" dxfId="7" priority="13" operator="containsText" text="error">
+      <formula>NOT(ISERROR(SEARCH("error",F27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="14" operator="containsText" text="not yet start">
+      <formula>NOT(ISERROR(SEARCH("not yet start",F27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="15" operator="containsText" text="pending">
+      <formula>NOT(ISERROR(SEARCH("pending",F27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="16" operator="containsText" text="done">
+      <formula>NOT(ISERROR(SEARCH("done",F27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F33:F39">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="error">
+      <formula>NOT(ISERROR(SEARCH("error",F33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="not yet start">
+      <formula>NOT(ISERROR(SEARCH("not yet start",F33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="pending">
+      <formula>NOT(ISERROR(SEARCH("pending",F33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="done">
+      <formula>NOT(ISERROR(SEARCH("done",F33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F10 F33:F39 F27:F29 F14:F23" xr:uid="{6AC56D31-3A4D-4D3B-BF31-CF83B6839E6A}">
+      <formula1>"done, pending, not yet start, error"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update on mobile token mechanism and new response structure for /dictionary/sync_all
</commit_message>
<xml_diff>
--- a/Notebook.xlsx
+++ b/Notebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phara\OneDrive\Desktop\FMIS\python\dictionary_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A44082-A36D-4101-B157-37CD8CE8921D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AC2952-8763-4E5C-A692-D31CEA6ABACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3984" yWindow="588" windowWidth="10980" windowHeight="11652" activeTab="1" xr2:uid="{486725EA-1341-4414-9EC0-725F2D77815B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{486725EA-1341-4414-9EC0-725F2D77815B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="71">
   <si>
     <t>No</t>
   </si>
@@ -243,6 +243,15 @@
   </si>
   <si>
     <t>- they want to keep deviceID so might save them all</t>
+  </si>
+  <si>
+    <t>POST /dictionary/staging/bulk_import/</t>
+  </si>
+  <si>
+    <t>POST /dictionary/staging/import_status/{task_id}/</t>
+  </si>
+  <si>
+    <t>GET /dictionary/template/</t>
   </si>
 </sst>
 </file>
@@ -444,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -473,6 +482,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -509,6 +527,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -526,15 +553,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1028,12 +1046,12 @@
       </c>
     </row>
     <row r="5" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="14"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="17"/>
     </row>
     <row r="6" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J6" s="1">
@@ -1153,12 +1171,12 @@
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="10:14" ht="24.6" x14ac:dyDescent="0.85">
-      <c r="J16" s="15" t="s">
+      <c r="J16" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="17"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="20"/>
     </row>
     <row r="17" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J17" s="1">
@@ -1235,12 +1253,12 @@
       <c r="M23" s="1"/>
     </row>
     <row r="24" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
-      <c r="J24" s="18" t="s">
+      <c r="J24" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="20"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="23"/>
     </row>
     <row r="25" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J25" s="1">
@@ -1307,10 +1325,10 @@
       <c r="M30" s="1"/>
     </row>
     <row r="31" spans="10:13" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="J31" s="21"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="23"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="26"/>
     </row>
     <row r="32" spans="10:13" ht="24.6" x14ac:dyDescent="0.85">
       <c r="J32" s="1">
@@ -1366,452 +1384,486 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F6179A3-1381-4E12-8A42-D0F2DF9F79BC}">
-  <dimension ref="B2:G39"/>
+  <dimension ref="B2:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="5" max="5" width="20.77734375" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="11" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="32"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
       <c r="G2" s="6" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B3" s="24"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="26"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
       <c r="G3" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="35"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="35"/>
       <c r="F5" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="35"/>
       <c r="F6" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="35"/>
       <c r="F7" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B8" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B9" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B10" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B11" s="30"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="32"/>
+    </row>
+    <row r="12" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B12" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
+    </row>
+    <row r="13" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B13" s="30"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
+    </row>
+    <row r="14" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B14" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B15" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B16" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B17" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B18" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B8" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B9" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B10" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B11" s="24"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="26"/>
-    </row>
-    <row r="12" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B12" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
-    </row>
-    <row r="13" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B13" s="24"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="26"/>
-    </row>
-    <row r="14" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B14" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B15" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B16" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B17" s="27" t="s">
+    <row r="19" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B19" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B18" s="27" t="s">
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B20" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B19" s="27" t="s">
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B21" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="6" t="s">
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B20" s="27" t="s">
+    <row r="22" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B22" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B21" s="27" t="s">
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B23" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="6" t="s">
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B22" s="27" t="s">
+    <row r="24" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B24" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B23" s="27" t="s">
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B25" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B26" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B24" s="24"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="26"/>
-    </row>
-    <row r="25" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B25" s="24" t="s">
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B27" s="30"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
+    </row>
+    <row r="28" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B28" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="26"/>
-    </row>
-    <row r="26" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B26" s="24"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="26"/>
-    </row>
-    <row r="27" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B27" s="27" t="s">
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="32"/>
+    </row>
+    <row r="29" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B29" s="30"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
+    </row>
+    <row r="30" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B30" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B28" s="27" t="s">
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B31" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B29" s="27" t="s">
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B32" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="26"/>
-    </row>
-    <row r="31" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B31" s="24" t="s">
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B33" s="30"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="32"/>
+    </row>
+    <row r="34" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B34" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="26"/>
-    </row>
-    <row r="32" spans="2:7" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="26"/>
-    </row>
-    <row r="33" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B33" s="27" t="s">
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="32"/>
+    </row>
+    <row r="35" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B35" s="30"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="32"/>
+    </row>
+    <row r="36" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B36" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B34" s="27" t="s">
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B37" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B35" s="27" t="s">
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B38" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B36" s="27" t="s">
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B39" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B37" s="27" t="s">
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B40" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B38" s="27" t="s">
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B41" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
-      <c r="B39" s="27" t="s">
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" ht="22.8" x14ac:dyDescent="0.8">
+      <c r="B42" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="10" t="s">
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="10" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B27:F27"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B20:E20"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F10">
     <cfRule type="containsText" dxfId="15" priority="25" operator="containsText" text="error">
@@ -1827,7 +1879,7 @@
       <formula>NOT(ISERROR(SEARCH("done",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F14:F23">
+  <conditionalFormatting sqref="F14:F26">
     <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="error">
       <formula>NOT(ISERROR(SEARCH("error",F14)))</formula>
     </cfRule>
@@ -1841,36 +1893,36 @@
       <formula>NOT(ISERROR(SEARCH("done",F14)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F27:F29">
+  <conditionalFormatting sqref="F30:F32">
     <cfRule type="containsText" dxfId="7" priority="13" operator="containsText" text="error">
-      <formula>NOT(ISERROR(SEARCH("error",F27)))</formula>
+      <formula>NOT(ISERROR(SEARCH("error",F30)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="14" operator="containsText" text="not yet start">
-      <formula>NOT(ISERROR(SEARCH("not yet start",F27)))</formula>
+      <formula>NOT(ISERROR(SEARCH("not yet start",F30)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="5" priority="15" operator="containsText" text="pending">
-      <formula>NOT(ISERROR(SEARCH("pending",F27)))</formula>
+      <formula>NOT(ISERROR(SEARCH("pending",F30)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="16" operator="containsText" text="done">
-      <formula>NOT(ISERROR(SEARCH("done",F27)))</formula>
+      <formula>NOT(ISERROR(SEARCH("done",F30)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F33:F39">
+  <conditionalFormatting sqref="F36:F42">
     <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="error">
-      <formula>NOT(ISERROR(SEARCH("error",F33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("error",F36)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="not yet start">
-      <formula>NOT(ISERROR(SEARCH("not yet start",F33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("not yet start",F36)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="pending">
-      <formula>NOT(ISERROR(SEARCH("pending",F33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("pending",F36)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="done">
-      <formula>NOT(ISERROR(SEARCH("done",F33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("done",F36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F10 F33:F39 F27:F29 F14:F23" xr:uid="{6AC56D31-3A4D-4D3B-BF31-CF83B6839E6A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F10 F36:F42 F30:F32 F14:F26" xr:uid="{6AC56D31-3A4D-4D3B-BF31-CF83B6839E6A}">
       <formula1>"done, pending, not yet start, error"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>